<commit_message>
Links for Switches and Keycaps
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tgmwien-my.sharepoint.com/personal/ljenkins_student_tgm_ac_at/Documents/WerkstaetteMacroPad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_AD4DB114E441178AC67DF45D5E10C16E683EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F04B5940-A44D-4B1C-933D-F2924B2EA038}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_AD4DB114E441178AC67DF45D5E10C16E683EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9156F4E6-1290-4066-8C22-124B5E031D58}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Produkt</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>https://amzn.eu/d/dTVjMqS</t>
+  </si>
+  <si>
+    <t>Keycaps</t>
+  </si>
+  <si>
+    <t>https://amzn.eu/d/jj6j4xa</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>https://amzn.eu/d/0HXf95k</t>
   </si>
 </sst>
 </file>
@@ -390,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,13 +456,31 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{75AA303B-0A20-4046-81C7-B649D6445D2E}"/>
     <hyperlink ref="C5" r:id="rId2" tooltip="https://amzn.eu/d/hbTjWBR" xr:uid="{5C14CC9B-5D1C-438F-9FB0-766D66F17C19}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{698D0168-0A83-4612-B29F-78E3C9B6FD50}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{55E58AC5-3929-4C28-BC2C-C3F6AE8F9CF0}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{FCCBAC27-846B-47BD-91DF-7342B8B5EC5C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished PCB i think
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tgmwien-my.sharepoint.com/personal/ljenkins_student_tgm_ac_at/Documents/WerkstaetteMacroPad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_AD4DB114E441178AC67DF45D5E10C16E683EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9156F4E6-1290-4066-8C22-124B5E031D58}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_AD4DB114E441178AC67DF45D5E10C16E683EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB91B23B-9C4C-4C3E-A18E-DFC53BABCC31}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added new Prices and estimated Final Price
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samih\Desktop\Schule\MacroPad\HEL_MacroPad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726CAEE0-C954-4E5D-94B3-9EE47251955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A227D6A-DC73-443A-983D-A20F7FC33D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Produkt</t>
   </si>
@@ -79,6 +90,15 @@
   </si>
   <si>
     <t>Kosten Gesamt</t>
+  </si>
+  <si>
+    <t>Keycaps Filament</t>
+  </si>
+  <si>
+    <t>1 Stück von Felix gespendet</t>
+  </si>
+  <si>
+    <t>Gesamtkosten pro Person (ohne Versandkst)</t>
   </si>
 </sst>
 </file>
@@ -407,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,6 +440,7 @@
     <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.5546875" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -446,14 +467,32 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>35.49</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>24.2</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
@@ -462,6 +501,12 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>7.55</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
@@ -486,8 +531,38 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="B8">
+        <v>0.37</v>
+      </c>
+      <c r="C8">
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <f>C8*B8</f>
+        <v>26.64</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>7.9164000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <f>(D9+D8+D5+D4+D3)/5</f>
+        <v>20.359280000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redesign, added buttons and rotary encoder
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tgmwien-my.sharepoint.com/personal/ljenkins_student_tgm_ac_at/Documents/WerkstaetteMacroPad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{8AB596D7-DCB8-46CA-A912-F0B5A85CA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE426691-88B7-4677-9CA0-2287574B1149}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{8AB596D7-DCB8-46CA-A912-F0B5A85CA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74FBA803-793E-4CAA-BC74-7B2F483EED1A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,6 +172,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +444,7 @@
   <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,9 +639,9 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="e">
-        <f>(SUM(B12D3:D13)/6)</f>
-        <v>#NAME?</v>
+      <c r="D14" s="2">
+        <f>(SUM(D3:D13)/6)</f>
+        <v>19.41333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Issue #32 (price of buttons cause div/0)
</commit_message>
<xml_diff>
--- a/Material.xlsx
+++ b/Material.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tgmwien-my.sharepoint.com/personal/ljenkins_student_tgm_ac_at/Documents/WerkstaetteMacroPad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{8AB596D7-DCB8-46CA-A912-F0B5A85CA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87B16698-89EC-44DE-BBDC-7BC5912A8075}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{8AB596D7-DCB8-46CA-A912-F0B5A85CA118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADDB1624-B424-41F5-BBA7-AB7F3FBD1F2C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -173,8 +173,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -187,10 +187,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,24 +452,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="57.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="56.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -499,7 +496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -527,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -552,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -577,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -602,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -627,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -652,44 +649,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D9/B9</f>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="e">
+      <c r="D10" s="2">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7600000000000002</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -711,7 +718,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -733,7 +740,7 @@
         <v>7.04</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
@@ -741,25 +748,93 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="2">
         <f>(SUM(F3:F13)/B19)</f>
-        <v>23.316666666666663</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23.776666666666667</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>